<commit_message>
Adding details to Getting Started
</commit_message>
<xml_diff>
--- a/data/exampleData/myodData/sampleMyodDataIndexTp-48_8_80.xlsx
+++ b/data/exampleData/myodData/sampleMyodDataIndexTp-48_8_80.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.17.109.24\internal_4dn\projects\4DNvestigator_data\myodData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindsly\Google Drive\UMICH\Research\4DNvesigator_lindsly\data\exampleData\myodData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="10515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="420" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>